<commit_message>
rewrite README; fill the grid about today's plan with right color; delete unused file.
</commit_message>
<xml_diff>
--- a/2020-21second.xlsx
+++ b/2020-21second.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AD7BED-F3C8-48D6-8AD4-91CAC6991323}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1周" sheetId="43" r:id="rId1"/>
@@ -28,17 +29,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'6周'!$B$2:$J$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'9周 '!$B$2:$J$22</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="I5" authorId="0" shapeId="0">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -54,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0">
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -70,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0">
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0">
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0" shapeId="0">
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -139,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0">
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -155,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0" shapeId="0">
+    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
         <r>
           <rPr>
@@ -171,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I13" authorId="0" shapeId="0">
+    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
       <text>
         <r>
           <rPr>
@@ -187,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I15" authorId="0" shapeId="0">
+    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
       <text>
         <r>
           <rPr>
@@ -203,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0" shapeId="0">
+    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -219,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0" shapeId="0">
+    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -235,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="0" shapeId="0">
+    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -277,12 +278,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -298,7 +299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -314,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -330,7 +331,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -346,7 +347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000005000000}">
       <text>
         <r>
           <rPr>
@@ -362,7 +363,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000006000000}">
       <text>
         <r>
           <rPr>
@@ -378,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0" shapeId="0">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000007000000}">
       <text>
         <r>
           <rPr>
@@ -394,7 +395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0">
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000008000000}">
       <text>
         <r>
           <rPr>
@@ -410,7 +411,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0">
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000009000000}">
       <text>
         <r>
           <rPr>
@@ -426,7 +427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -442,7 +443,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0">
+    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -458,7 +459,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0">
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -475,7 +476,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -491,7 +492,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -507,7 +508,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -544,7 +545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0">
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000010000000}">
       <text>
         <r>
           <rPr>
@@ -586,7 +587,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000011000000}">
       <text>
         <r>
           <rPr>
@@ -602,7 +603,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000012000000}">
       <text>
         <r>
           <rPr>
@@ -618,7 +619,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H10" authorId="0" shapeId="0">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000013000000}">
       <text>
         <r>
           <rPr>
@@ -634,7 +635,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0" shapeId="0">
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000014000000}">
       <text>
         <r>
           <rPr>
@@ -650,7 +651,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0">
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000015000000}">
       <text>
         <r>
           <rPr>
@@ -666,7 +667,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0" shapeId="0">
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000016000000}">
       <text>
         <r>
           <rPr>
@@ -682,7 +683,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0" shapeId="0">
+    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000017000000}">
       <text>
         <r>
           <rPr>
@@ -698,7 +699,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0">
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000018000000}">
       <text>
         <r>
           <rPr>
@@ -714,7 +715,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000019000000}">
       <text>
         <r>
           <rPr>
@@ -730,7 +731,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0" shapeId="0">
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -746,7 +747,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H12" authorId="0" shapeId="0">
+    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -762,7 +763,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0" shapeId="0">
+    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -778,7 +779,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G13" authorId="0" shapeId="0">
+    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -794,7 +795,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H13" authorId="0" shapeId="0">
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -810,7 +811,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I13" authorId="0" shapeId="0">
+    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -826,7 +827,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0">
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000020000000}">
       <text>
         <r>
           <rPr>
@@ -842,7 +843,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0" shapeId="0">
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000021000000}">
       <text>
         <r>
           <rPr>
@@ -858,7 +859,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H14" authorId="0" shapeId="0">
+    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000022000000}">
       <text>
         <r>
           <rPr>
@@ -874,7 +875,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I14" authorId="0" shapeId="0">
+    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000023000000}">
       <text>
         <r>
           <rPr>
@@ -890,7 +891,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H15" authorId="0" shapeId="0">
+    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000024000000}">
       <text>
         <r>
           <rPr>
@@ -906,7 +907,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I15" authorId="0" shapeId="0">
+    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000025000000}">
       <text>
         <r>
           <rPr>
@@ -923,7 +924,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0" shapeId="0">
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000026000000}">
       <text>
         <r>
           <rPr>
@@ -939,7 +940,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0" shapeId="0">
+    <comment ref="G16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000027000000}">
       <text>
         <r>
           <rPr>
@@ -955,7 +956,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H16" authorId="0" shapeId="0">
+    <comment ref="H16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000028000000}">
       <text>
         <r>
           <rPr>
@@ -971,7 +972,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0" shapeId="0">
+    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000029000000}">
       <text>
         <r>
           <rPr>
@@ -987,7 +988,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0" shapeId="0">
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002A000000}">
       <text>
         <r>
           <rPr>
@@ -1003,7 +1004,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G17" authorId="0" shapeId="0">
+    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002B000000}">
       <text>
         <r>
           <rPr>
@@ -1019,7 +1020,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H17" authorId="0" shapeId="0">
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002C000000}">
       <text>
         <r>
           <rPr>
@@ -1035,7 +1036,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0" shapeId="0">
+    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002D000000}">
       <text>
         <r>
           <rPr>
@@ -1051,7 +1052,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="0" shapeId="0">
+    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002E000000}">
       <text>
         <r>
           <rPr>
@@ -1067,7 +1068,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="0" shapeId="0">
+    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002F000000}">
       <text>
         <r>
           <rPr>
@@ -1083,7 +1084,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0" shapeId="0">
+    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000030000000}">
       <text>
         <r>
           <rPr>
@@ -1099,7 +1100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C19" authorId="0" shapeId="0">
+    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000031000000}">
       <text>
         <r>
           <rPr>
@@ -1115,7 +1116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G19" authorId="0" shapeId="0">
+    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000032000000}">
       <text>
         <r>
           <rPr>
@@ -1131,7 +1132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0">
+    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000033000000}">
       <text>
         <r>
           <rPr>
@@ -1147,7 +1148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="0" shapeId="0">
+    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000034000000}">
       <text>
         <r>
           <rPr>
@@ -1163,7 +1164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C20" authorId="0" shapeId="0">
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000035000000}">
       <text>
         <r>
           <rPr>
@@ -1189,7 +1190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0" shapeId="0">
+    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000036000000}">
       <text>
         <r>
           <rPr>
@@ -1205,7 +1206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H20" authorId="0" shapeId="0">
+    <comment ref="H20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000037000000}">
       <text>
         <r>
           <rPr>
@@ -1221,7 +1222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I20" authorId="0" shapeId="0">
+    <comment ref="I20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000038000000}">
       <text>
         <r>
           <rPr>
@@ -1242,12 +1243,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1263,7 +1264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1279,7 +1280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1295,7 +1296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1311,7 +1312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1327,7 +1328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1343,7 +1344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1359,7 +1360,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000008000000}">
       <text>
         <r>
           <rPr>
@@ -1375,7 +1376,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000009000000}">
       <text>
         <r>
           <rPr>
@@ -1391,7 +1392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -1407,7 +1408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -1423,7 +1424,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0" shapeId="0">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -1439,7 +1440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0" shapeId="0">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -1455,7 +1456,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0">
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -1471,7 +1472,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0">
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -1487,7 +1488,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0">
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000010000000}">
       <text>
         <r>
           <rPr>
@@ -1503,7 +1504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000011000000}">
       <text>
         <r>
           <rPr>
@@ -1519,7 +1520,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000012000000}">
       <text>
         <r>
           <rPr>
@@ -1535,7 +1536,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000013000000}">
       <text>
         <r>
           <rPr>
@@ -1551,7 +1552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="0" shapeId="0">
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000014000000}">
       <text>
         <r>
           <rPr>
@@ -1567,7 +1568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0">
+    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000015000000}">
       <text>
         <r>
           <rPr>
@@ -1583,7 +1584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0">
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000016000000}">
       <text>
         <r>
           <rPr>
@@ -1600,7 +1601,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000017000000}">
       <text>
         <r>
           <rPr>
@@ -1616,7 +1617,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0" shapeId="0">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000018000000}">
       <text>
         <r>
           <rPr>
@@ -1632,7 +1633,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000019000000}">
       <text>
         <r>
           <rPr>
@@ -1648,7 +1649,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0">
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -1664,7 +1665,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -1680,7 +1681,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -1717,7 +1718,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -1733,7 +1734,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0">
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -1749,7 +1750,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0">
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -1791,7 +1792,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000020000000}">
       <text>
         <r>
           <rPr>
@@ -1807,7 +1808,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000021000000}">
       <text>
         <r>
           <rPr>
@@ -1823,7 +1824,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000022000000}">
       <text>
         <r>
           <rPr>
@@ -1839,7 +1840,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0">
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000023000000}">
       <text>
         <r>
           <rPr>
@@ -1855,7 +1856,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000024000000}">
       <text>
         <r>
           <rPr>
@@ -1871,7 +1872,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H10" authorId="0" shapeId="0">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000025000000}">
       <text>
         <r>
           <rPr>
@@ -1887,7 +1888,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0" shapeId="0">
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000026000000}">
       <text>
         <r>
           <rPr>
@@ -1903,7 +1904,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0">
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000027000000}">
       <text>
         <r>
           <rPr>
@@ -1919,7 +1920,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0">
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000028000000}">
       <text>
         <r>
           <rPr>
@@ -1935,7 +1936,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0">
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000029000000}">
       <text>
         <r>
           <rPr>
@@ -1951,7 +1952,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0" shapeId="0">
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00002A000000}">
       <text>
         <r>
           <rPr>
@@ -1967,7 +1968,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0" shapeId="0">
+    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00002B000000}">
       <text>
         <r>
           <rPr>
@@ -1983,7 +1984,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0">
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00002C000000}">
       <text>
         <r>
           <rPr>
@@ -1999,7 +2000,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00002D000000}">
       <text>
         <r>
           <rPr>
@@ -2015,7 +2016,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00002E000000}">
       <text>
         <r>
           <rPr>
@@ -2031,7 +2032,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0" shapeId="0">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00002F000000}">
       <text>
         <r>
           <rPr>
@@ -2047,7 +2048,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000030000000}">
       <text>
         <r>
           <rPr>
@@ -2063,7 +2064,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0" shapeId="0">
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000031000000}">
       <text>
         <r>
           <rPr>
@@ -2079,7 +2080,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H12" authorId="0" shapeId="0">
+    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000032000000}">
       <text>
         <r>
           <rPr>
@@ -2095,7 +2096,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0" shapeId="0">
+    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000033000000}">
       <text>
         <r>
           <rPr>
@@ -2111,7 +2112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0">
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000034000000}">
       <text>
         <r>
           <rPr>
@@ -2127,7 +2128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0" shapeId="0">
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000035000000}">
       <text>
         <r>
           <rPr>
@@ -2143,7 +2144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="0" shapeId="0">
+    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000036000000}">
       <text>
         <r>
           <rPr>
@@ -2159,7 +2160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="0" shapeId="0">
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000037000000}">
       <text>
         <r>
           <rPr>
@@ -2175,7 +2176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G13" authorId="0" shapeId="0">
+    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000038000000}">
       <text>
         <r>
           <rPr>
@@ -2191,7 +2192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H13" authorId="0" shapeId="0">
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000039000000}">
       <text>
         <r>
           <rPr>
@@ -2207,7 +2208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I13" authorId="0" shapeId="0">
+    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00003A000000}">
       <text>
         <r>
           <rPr>
@@ -2223,7 +2224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0">
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00003B000000}">
       <text>
         <r>
           <rPr>
@@ -2239,7 +2240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="0" shapeId="0">
+    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00003C000000}">
       <text>
         <r>
           <rPr>
@@ -2255,7 +2256,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0" shapeId="0">
+    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00003D000000}">
       <text>
         <r>
           <rPr>
@@ -2271,7 +2272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0" shapeId="0">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00003E000000}">
       <text>
         <r>
           <rPr>
@@ -2287,7 +2288,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0" shapeId="0">
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00003F000000}">
       <text>
         <r>
           <rPr>
@@ -2303,7 +2304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H14" authorId="0" shapeId="0">
+    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000040000000}">
       <text>
         <r>
           <rPr>
@@ -2319,7 +2320,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I14" authorId="0" shapeId="0">
+    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000041000000}">
       <text>
         <r>
           <rPr>
@@ -2335,7 +2336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H15" authorId="0" shapeId="0">
+    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000042000000}">
       <text>
         <r>
           <rPr>
@@ -2351,7 +2352,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I15" authorId="0" shapeId="0">
+    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000043000000}">
       <text>
         <r>
           <rPr>
@@ -2368,7 +2369,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0" shapeId="0">
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000044000000}">
       <text>
         <r>
           <rPr>
@@ -2384,7 +2385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D16" authorId="0" shapeId="0">
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000045000000}">
       <text>
         <r>
           <rPr>
@@ -2400,7 +2401,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0" shapeId="0">
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000046000000}">
       <text>
         <r>
           <rPr>
@@ -2416,7 +2417,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0" shapeId="0">
+    <comment ref="G16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000047000000}">
       <text>
         <r>
           <rPr>
@@ -2432,7 +2433,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H16" authorId="0" shapeId="0">
+    <comment ref="H16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000048000000}">
       <text>
         <r>
           <rPr>
@@ -2448,7 +2449,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0" shapeId="0">
+    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000049000000}">
       <text>
         <r>
           <rPr>
@@ -2464,7 +2465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0" shapeId="0">
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00004A000000}">
       <text>
         <r>
           <rPr>
@@ -2480,7 +2481,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0" shapeId="0">
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00004B000000}">
       <text>
         <r>
           <rPr>
@@ -2496,7 +2497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G17" authorId="0" shapeId="0">
+    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00004C000000}">
       <text>
         <r>
           <rPr>
@@ -2512,7 +2513,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H17" authorId="0" shapeId="0">
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00004D000000}">
       <text>
         <r>
           <rPr>
@@ -2528,7 +2529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0" shapeId="0">
+    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00004E000000}">
       <text>
         <r>
           <rPr>
@@ -2544,7 +2545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="0" shapeId="0">
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00004F000000}">
       <text>
         <r>
           <rPr>
@@ -2560,7 +2561,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E18" authorId="0" shapeId="0">
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000050000000}">
       <text>
         <r>
           <rPr>
@@ -2576,7 +2577,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0" shapeId="0">
+    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000051000000}">
       <text>
         <r>
           <rPr>
@@ -2592,7 +2593,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="0" shapeId="0">
+    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000052000000}">
       <text>
         <r>
           <rPr>
@@ -2608,7 +2609,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="0" shapeId="0">
+    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000053000000}">
       <text>
         <r>
           <rPr>
@@ -2624,7 +2625,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0" shapeId="0">
+    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000054000000}">
       <text>
         <r>
           <rPr>
@@ -2640,7 +2641,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C19" authorId="0" shapeId="0">
+    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000055000000}">
       <text>
         <r>
           <rPr>
@@ -2656,7 +2657,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E19" authorId="0" shapeId="0">
+    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000056000000}">
       <text>
         <r>
           <rPr>
@@ -2672,7 +2673,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="0" shapeId="0">
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000057000000}">
       <text>
         <r>
           <rPr>
@@ -2688,7 +2689,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G19" authorId="0" shapeId="0">
+    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000058000000}">
       <text>
         <r>
           <rPr>
@@ -2704,7 +2705,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0">
+    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000059000000}">
       <text>
         <r>
           <rPr>
@@ -2720,7 +2721,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="0" shapeId="0">
+    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00005A000000}">
       <text>
         <r>
           <rPr>
@@ -2736,7 +2737,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C20" authorId="0" shapeId="0">
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00005B000000}">
       <text>
         <r>
           <rPr>
@@ -2752,7 +2753,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0">
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00005C000000}">
       <text>
         <r>
           <rPr>
@@ -2768,7 +2769,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0">
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00005D000000}">
       <text>
         <r>
           <rPr>
@@ -2784,7 +2785,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0" shapeId="0">
+    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00005E000000}">
       <text>
         <r>
           <rPr>
@@ -2805,12 +2806,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0" shapeId="0">
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -2826,7 +2827,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -2842,7 +2843,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
       <text>
         <r>
           <rPr>
@@ -2858,7 +2859,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0">
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
       <text>
         <r>
           <rPr>
@@ -2874,7 +2875,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
       <text>
         <r>
           <rPr>
@@ -2890,7 +2891,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000006000000}">
       <text>
         <r>
           <rPr>
@@ -2906,7 +2907,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000007000000}">
       <text>
         <r>
           <rPr>
@@ -2922,7 +2923,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000008000000}">
       <text>
         <r>
           <rPr>
@@ -2938,7 +2939,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000009000000}">
       <text>
         <r>
           <rPr>
@@ -2954,7 +2955,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -2970,7 +2971,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -2986,7 +2987,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0" shapeId="0">
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -3002,7 +3003,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0" shapeId="0">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -3018,7 +3019,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0">
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -3034,7 +3035,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0">
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -3050,7 +3051,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0">
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000010000000}">
       <text>
         <r>
           <rPr>
@@ -3087,7 +3088,39 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{73E161C9-2E85-47BA-A021-8842B7C97393}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+尝试非周期方向，各种尝试。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{B243C8A6-BAFB-4ECB-8349-4F4A49FA1F46}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+尝试非周期方向，各种尝试。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000011000000}">
       <text>
         <r>
           <rPr>
@@ -3124,7 +3157,39 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{C558CCFF-D288-4C59-9F45-12C2FDB369DC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+尝试非周期方向，各种尝试。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{9D04EB6E-6470-4E02-9A9E-1023E054A0DC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+尝试非周期方向，各种尝试。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000012000000}">
       <text>
         <r>
           <rPr>
@@ -3140,7 +3205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000013000000}">
       <text>
         <r>
           <rPr>
@@ -3156,7 +3221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0">
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000014000000}">
       <text>
         <r>
           <rPr>
@@ -3172,7 +3237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000015000000}">
       <text>
         <r>
           <rPr>
@@ -3188,7 +3253,55 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{D46F7D6A-E363-4DEE-9A8C-5F6F779B6667}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+处理一下文献翻译，最后勘误。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000017000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+还是那篇综述。一口气翻译完吧。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000018000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+得去1教进行开题报告。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000019000000}">
       <text>
         <r>
           <rPr>
@@ -3204,23 +3317,71 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-还是那篇综述。一口气翻译完吧。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F10" authorId="0" shapeId="0">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00001A000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+神界：原罪2，太好玩了，一支玩下去吧!以后的每周都玩这个。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00001B000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+还是玩那个游戏。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00001C000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+可能要讨论多一会儿。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{A9059024-5895-4F21-8FEC-07A1B1501261}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+做好最后的准备就上传吧！</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -3236,7 +3397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0">
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -3252,7 +3413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H10" authorId="0" shapeId="0">
+    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000020000000}">
       <text>
         <r>
           <rPr>
@@ -3268,7 +3429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0" shapeId="0">
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000021000000}">
       <text>
         <r>
           <rPr>
@@ -3284,23 +3445,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-可能要讨论多一会儿。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D11" authorId="0" shapeId="0">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{4E890EBE-FBF4-42B9-846C-32B34D3DD992}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+讨论完了就去实现一些代码。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000023000000}">
       <text>
         <r>
           <rPr>
@@ -3316,23 +3477,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-得去1教进行开题报告。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G11" authorId="0" shapeId="0">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000024000000}">
       <text>
         <r>
           <rPr>
@@ -3348,23 +3493,39 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-神界：原罪2，太好玩了，一支玩下去吧!以后的每周都玩这个。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I11" authorId="0" shapeId="0">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000025000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+尝试非周期方向，各种尝试。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000026000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+尝试非周期方向，各种尝试。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000027000000}">
       <text>
         <r>
           <rPr>
@@ -3380,23 +3541,39 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-开始构思论文，如果讨论的结果很满意的话。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D12" authorId="0" shapeId="0">
+    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000028000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+还是玩那个游戏。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{277309F2-30DC-4FCB-A3B5-3B6CFDDBAB61}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+八卦去了。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000029000000}">
       <text>
         <r>
           <rPr>
@@ -3412,7 +3589,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0" shapeId="0">
+    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00002A000000}">
       <text>
         <r>
           <rPr>
@@ -3428,7 +3605,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0">
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00002B000000}">
       <text>
         <r>
           <rPr>
@@ -3444,7 +3621,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0" shapeId="0">
+    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00002C000000}">
       <text>
         <r>
           <rPr>
@@ -3460,7 +3637,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H12" authorId="0" shapeId="0">
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00002D000000}">
       <text>
         <r>
           <rPr>
@@ -3476,7 +3653,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0" shapeId="0">
+    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00002E000000}">
       <text>
         <r>
           <rPr>
@@ -3492,7 +3669,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0" shapeId="0">
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{7872573E-29A9-4B86-B1DD-9683A03FD836}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+八卦去了。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00002F000000}">
       <text>
         <r>
           <rPr>
@@ -3508,7 +3701,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="0" shapeId="0">
+    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000030000000}">
       <text>
         <r>
           <rPr>
@@ -3524,7 +3717,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="0" shapeId="0">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000031000000}">
       <text>
         <r>
           <rPr>
@@ -3540,7 +3733,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G13" authorId="0" shapeId="0">
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000032000000}">
       <text>
         <r>
           <rPr>
@@ -3556,7 +3749,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H13" authorId="0" shapeId="0">
+    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000033000000}">
       <text>
         <r>
           <rPr>
@@ -3572,7 +3765,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I13" authorId="0" shapeId="0">
+    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000034000000}">
       <text>
         <r>
           <rPr>
@@ -3588,103 +3781,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-尝试非周期方向，各种尝试。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E14" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-尝试非周期方向，各种尝试。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F14" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-尝试非周期方向，各种尝试。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G14" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-尝试非周期方向，各种尝试。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H14" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-还是玩那个游戏。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I14" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-还是玩那个游戏。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I15" authorId="0" shapeId="0">
+    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000035000000}">
       <text>
         <r>
           <rPr>
@@ -3701,7 +3798,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="D16" authorId="0" shapeId="0">
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{755D3773-871E-4493-A4CB-E67E905F830B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+完成了新的小量推导。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000036000000}">
       <text>
         <r>
           <rPr>
@@ -3717,7 +3830,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0" shapeId="0">
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000037000000}">
       <text>
         <r>
           <rPr>
@@ -3733,7 +3846,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0" shapeId="0">
+    <comment ref="G16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000038000000}">
       <text>
         <r>
           <rPr>
@@ -3749,7 +3862,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H16" authorId="0" shapeId="0">
+    <comment ref="H16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000039000000}">
       <text>
         <r>
           <rPr>
@@ -3765,7 +3878,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0" shapeId="0">
+    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00003A000000}">
       <text>
         <r>
           <rPr>
@@ -3781,7 +3894,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0" shapeId="0">
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{A951F08F-EC50-4584-A17D-47B20FDBF644}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+完成了新的小量推导。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00003B000000}">
       <text>
         <r>
           <rPr>
@@ -3797,7 +3926,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="0" shapeId="0">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00003C000000}">
       <text>
         <r>
           <rPr>
@@ -3813,7 +3942,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G17" authorId="0" shapeId="0">
+    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00003D000000}">
       <text>
         <r>
           <rPr>
@@ -3829,7 +3958,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H17" authorId="0" shapeId="0">
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00003E000000}">
       <text>
         <r>
           <rPr>
@@ -3845,7 +3974,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0" shapeId="0">
+    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00003F000000}">
       <text>
         <r>
           <rPr>
@@ -3861,7 +3990,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="0" shapeId="0">
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000040000000}">
       <text>
         <r>
           <rPr>
@@ -3877,7 +4006,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E18" authorId="0" shapeId="0">
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000041000000}">
       <text>
         <r>
           <rPr>
@@ -3893,7 +4022,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0" shapeId="0">
+    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000042000000}">
       <text>
         <r>
           <rPr>
@@ -3909,7 +4038,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="0" shapeId="0">
+    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000043000000}">
       <text>
         <r>
           <rPr>
@@ -3925,7 +4054,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="0" shapeId="0">
+    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000044000000}">
       <text>
         <r>
           <rPr>
@@ -3941,7 +4070,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0" shapeId="0">
+    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000045000000}">
       <text>
         <r>
           <rPr>
@@ -3957,7 +4086,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="E19" authorId="0" shapeId="0">
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{AECCB75A-6506-4A14-89C1-40F5223FF2B7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+洗那双白鞋子。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000046000000}">
       <text>
         <r>
           <rPr>
@@ -3973,7 +4118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="0" shapeId="0">
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000047000000}">
       <text>
         <r>
           <rPr>
@@ -3989,7 +4134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G19" authorId="0" shapeId="0">
+    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000048000000}">
       <text>
         <r>
           <rPr>
@@ -4005,7 +4150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0">
+    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000049000000}">
       <text>
         <r>
           <rPr>
@@ -4021,7 +4166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="0" shapeId="0">
+    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00004A000000}">
       <text>
         <r>
           <rPr>
@@ -4037,7 +4182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0">
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00004B000000}">
       <text>
         <r>
           <rPr>
@@ -4053,7 +4198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0">
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00004C000000}">
       <text>
         <r>
           <rPr>
@@ -4069,7 +4214,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0" shapeId="0">
+    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00004D000000}">
       <text>
         <r>
           <rPr>
@@ -4090,7 +4235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="114">
   <si>
     <t>起床吃饭</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4541,10 +4686,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>论文构思</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>写论文</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -4564,7 +4705,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="26">
     <font>
       <sz val="11"/>
@@ -5390,7 +5531,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5755,6 +5896,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5765,7 +5909,7 @@
   <cellStyles count="3">
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="样式 1" xfId="2"/>
+    <cellStyle name="样式 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -5998,25 +6142,25 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.82352941176470584</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.88235294117647056</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.94117647058823528</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.94117647058823528</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.94117647058823528</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.76470588235294112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6420,25 +6564,25 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.88235294117647056</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.88235294117647056</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.88235294117647056</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.76470588235294112</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.76470588235294112</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.52941176470588236</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.94117647058823528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6842,25 +6986,25 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.88235294117647056</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.82352941176470584</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.82352941176470584</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.70588235294117652</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.76470588235294112</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.76470588235294112</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7264,25 +7408,25 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.82352941176470584</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.88235294117647056</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.88235294117647056</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.94117647058823528</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.70588235294117652</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.6470588235294118</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.94117647058823528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7686,25 +7830,25 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.94444444444444442</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.88888888888888884</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.55555555555555558</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8108,19 +8252,19 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.88888888888888884</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.77777777777777779</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.22222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -8476,7 +8620,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8531,7 +8674,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.72222222222222221</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -8901,7 +9044,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.89915966386554635</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -8937,7 +9080,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.89915966386554635</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -14501,14 +14644,12 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
-      <sheetName val="gcolor"/>
     </sheetNames>
     <definedNames>
       <definedName name="GetColor"/>
     </definedNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -14590,6 +14731,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -14625,6 +14783,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -14800,7 +14975,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O23"/>
   <sheetViews>
@@ -15407,40 +15582,40 @@
     </row>
     <row r="20" spans="1:15" ht="16.5">
       <c r="A20" s="46"/>
-      <c r="B20" s="126" t="s">
+      <c r="B20" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="42" t="e">
+      <c r="C20" s="42">
         <f ca="1">[1]!GetColor(K6,C3:C19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D20" s="42" t="e">
+        <v>14</v>
+      </c>
+      <c r="D20" s="42">
         <f ca="1">[1]!GetColor(K6,D3:D19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E20" s="42" t="e">
+        <v>15</v>
+      </c>
+      <c r="E20" s="42">
         <f ca="1">[1]!GetColor(K6,E3:E19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F20" s="42" t="e">
+        <v>17</v>
+      </c>
+      <c r="F20" s="42">
         <f ca="1">[1]!GetColor(K6,F3:F19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G20" s="42" t="e">
+        <v>16</v>
+      </c>
+      <c r="G20" s="42">
         <f ca="1">[1]!GetColor(K6,G3:G19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H20" s="42" t="e">
+        <v>16</v>
+      </c>
+      <c r="H20" s="42">
         <f ca="1">[1]!GetColor(K6,H3:H19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I20" s="42" t="e">
+        <v>16</v>
+      </c>
+      <c r="I20" s="42">
         <f ca="1">[1]!GetColor(K6,I3:I19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J20" s="43" t="e">
+        <v>13</v>
+      </c>
+      <c r="J20" s="43">
         <f ca="1">SUM(C20:I20)</f>
-        <v>#NAME?</v>
+        <v>107</v>
       </c>
       <c r="K20" s="6"/>
       <c r="M20" s="2"/>
@@ -15448,38 +15623,38 @@
     </row>
     <row r="21" spans="1:15" ht="17.25" thickBot="1">
       <c r="A21" s="46"/>
-      <c r="B21" s="127"/>
-      <c r="C21" s="44" t="e">
+      <c r="B21" s="128"/>
+      <c r="C21" s="44">
         <f ca="1">C20/COUNTA(C3:C19)*100%</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D21" s="44" t="e">
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="D21" s="44">
         <f t="shared" ref="D21:I21" ca="1" si="0">D20/COUNTA(D3:D19)*100%</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E21" s="44" t="e">
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="E21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="F21" s="44" t="e">
+        <v>1</v>
+      </c>
+      <c r="F21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G21" s="44" t="e">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="G21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H21" s="44" t="e">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="H21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I21" s="44" t="e">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="I21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="J21" s="45" t="e">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="J21" s="45">
         <f ca="1">AVERAGE(C21:I21)</f>
-        <v>#NAME?</v>
+        <v>0.89915966386554635</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="3"/>
@@ -15532,7 +15707,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -16138,40 +16313,40 @@
     </row>
     <row r="20" spans="1:15" ht="16.5">
       <c r="A20" s="46"/>
-      <c r="B20" s="126" t="s">
+      <c r="B20" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="42" t="e">
+      <c r="C20" s="42">
         <f ca="1">[1]!GetColor(K6,C3:C19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D20" s="42" t="e">
+        <v>15</v>
+      </c>
+      <c r="D20" s="42">
         <f ca="1">[1]!GetColor(K6,D3:D19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E20" s="42" t="e">
+        <v>15</v>
+      </c>
+      <c r="E20" s="42">
         <f ca="1">[1]!GetColor(K6,E3:E19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F20" s="42" t="e">
+        <v>15</v>
+      </c>
+      <c r="F20" s="42">
         <f ca="1">[1]!GetColor(K6,F3:F19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G20" s="42" t="e">
+        <v>13</v>
+      </c>
+      <c r="G20" s="42">
         <f ca="1">[1]!GetColor(K6,G3:G19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H20" s="42" t="e">
+        <v>13</v>
+      </c>
+      <c r="H20" s="42">
         <f ca="1">[1]!GetColor(K6,H3:H19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I20" s="42" t="e">
+        <v>9</v>
+      </c>
+      <c r="I20" s="42">
         <f ca="1">[1]!GetColor(K6,I3:I19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J20" s="43" t="e">
+        <v>16</v>
+      </c>
+      <c r="J20" s="43">
         <f ca="1">SUM(C20:I20)</f>
-        <v>#NAME?</v>
+        <v>96</v>
       </c>
       <c r="K20" s="6"/>
       <c r="M20" s="2"/>
@@ -16179,38 +16354,38 @@
     </row>
     <row r="21" spans="1:15" ht="17.25" thickBot="1">
       <c r="A21" s="46"/>
-      <c r="B21" s="127"/>
-      <c r="C21" s="44" t="e">
+      <c r="B21" s="128"/>
+      <c r="C21" s="44">
         <f ca="1">C20/COUNTA(C3:C19)*100%</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D21" s="44" t="e">
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="D21" s="44">
         <f t="shared" ref="D21:I21" ca="1" si="0">D20/COUNTA(D3:D19)*100%</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E21" s="44" t="e">
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="E21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="F21" s="44" t="e">
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="F21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G21" s="44" t="e">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="G21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H21" s="44" t="e">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="H21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I21" s="44" t="e">
+        <v>0.52941176470588236</v>
+      </c>
+      <c r="I21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="J21" s="45" t="e">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="J21" s="45">
         <f ca="1">AVERAGE(C21:I21)</f>
-        <v>#NAME?</v>
+        <v>0.80672268907563016</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="3"/>
@@ -16263,7 +16438,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -16869,40 +17044,40 @@
     </row>
     <row r="20" spans="1:22" ht="16.5">
       <c r="A20" s="46"/>
-      <c r="B20" s="126" t="s">
+      <c r="B20" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="42" t="e">
+      <c r="C20" s="42">
         <f ca="1">[1]!GetColor(K6,C3:C19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D20" s="42" t="e">
+        <v>15</v>
+      </c>
+      <c r="D20" s="42">
         <f ca="1">[1]!GetColor(K6,D3:D19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E20" s="42" t="e">
+        <v>14</v>
+      </c>
+      <c r="E20" s="42">
         <f ca="1">[1]!GetColor(K6,E3:E19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F20" s="42" t="e">
+        <v>14</v>
+      </c>
+      <c r="F20" s="42">
         <f ca="1">[1]!GetColor(K6,F3:F19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G20" s="42" t="e">
+        <v>12</v>
+      </c>
+      <c r="G20" s="42">
         <f ca="1">[1]!GetColor(K6,G3:G19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H20" s="42" t="e">
+        <v>13</v>
+      </c>
+      <c r="H20" s="42">
         <f ca="1">[1]!GetColor(K6,H3:H19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I20" s="42" t="e">
+        <v>13</v>
+      </c>
+      <c r="I20" s="42">
         <f ca="1">[1]!GetColor(K6,I3:I19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J20" s="43" t="e">
+        <v>17</v>
+      </c>
+      <c r="J20" s="43">
         <f ca="1">SUM(C20:I20)</f>
-        <v>#NAME?</v>
+        <v>98</v>
       </c>
       <c r="K20" s="6"/>
       <c r="M20" s="2"/>
@@ -16910,38 +17085,38 @@
     </row>
     <row r="21" spans="1:22" ht="17.25" thickBot="1">
       <c r="A21" s="46"/>
-      <c r="B21" s="127"/>
-      <c r="C21" s="44" t="e">
+      <c r="B21" s="128"/>
+      <c r="C21" s="44">
         <f ca="1">C20/COUNTA(C3:C19)*100%</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D21" s="44" t="e">
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="D21" s="44">
         <f t="shared" ref="D21:I21" ca="1" si="0">D20/COUNTA(D3:D19)*100%</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E21" s="44" t="e">
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="E21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="F21" s="44" t="e">
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="F21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G21" s="44" t="e">
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="G21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H21" s="44" t="e">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="H21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I21" s="44" t="e">
+        <v>0.76470588235294112</v>
+      </c>
+      <c r="I21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="J21" s="45" t="e">
+        <v>1</v>
+      </c>
+      <c r="J21" s="45">
         <f ca="1">AVERAGE(C21:I21)</f>
-        <v>#NAME?</v>
+        <v>0.82352941176470584</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="3"/>
@@ -17007,7 +17182,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
@@ -17612,40 +17787,40 @@
     </row>
     <row r="20" spans="1:22" ht="16.5">
       <c r="A20" s="46"/>
-      <c r="B20" s="126" t="s">
+      <c r="B20" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="42" t="e">
+      <c r="C20" s="42">
         <f ca="1">[1]!GetColor(K6,C3:C19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D20" s="42" t="e">
+        <v>14</v>
+      </c>
+      <c r="D20" s="42">
         <f ca="1">[1]!GetColor(K6,D3:D19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E20" s="42" t="e">
+        <v>15</v>
+      </c>
+      <c r="E20" s="42">
         <f ca="1">[1]!GetColor(K6,E3:E19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F20" s="42" t="e">
+        <v>15</v>
+      </c>
+      <c r="F20" s="42">
         <f ca="1">[1]!GetColor(K6,F3:F19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G20" s="42" t="e">
+        <v>16</v>
+      </c>
+      <c r="G20" s="42">
         <f ca="1">[1]!GetColor(K6,G3:G19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H20" s="42" t="e">
+        <v>12</v>
+      </c>
+      <c r="H20" s="42">
         <f ca="1">[1]!GetColor(K6,H3:H19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I20" s="42" t="e">
+        <v>11</v>
+      </c>
+      <c r="I20" s="42">
         <f ca="1">[1]!GetColor(K6,I3:I19, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J20" s="43" t="e">
+        <v>16</v>
+      </c>
+      <c r="J20" s="43">
         <f ca="1">SUM(C20:I20)</f>
-        <v>#NAME?</v>
+        <v>99</v>
       </c>
       <c r="K20" s="6"/>
       <c r="M20" s="2"/>
@@ -17653,38 +17828,38 @@
     </row>
     <row r="21" spans="1:22" ht="17.25" thickBot="1">
       <c r="A21" s="46"/>
-      <c r="B21" s="127"/>
-      <c r="C21" s="44" t="e">
+      <c r="B21" s="128"/>
+      <c r="C21" s="44">
         <f ca="1">C20/COUNTA(C3:C19)*100%</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D21" s="44" t="e">
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="D21" s="44">
         <f t="shared" ref="D21:I21" ca="1" si="0">D20/COUNTA(D3:D19)*100%</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E21" s="44" t="e">
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="E21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="F21" s="44" t="e">
+        <v>0.88235294117647056</v>
+      </c>
+      <c r="F21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G21" s="44" t="e">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="G21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H21" s="44" t="e">
+        <v>0.70588235294117652</v>
+      </c>
+      <c r="H21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I21" s="44" t="e">
+        <v>0.6470588235294118</v>
+      </c>
+      <c r="I21" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="J21" s="45" t="e">
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="J21" s="45">
         <f ca="1">AVERAGE(C21:I21)</f>
-        <v>#NAME?</v>
+        <v>0.83193277310924374</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="3"/>
@@ -17751,7 +17926,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
@@ -18388,40 +18563,40 @@
     </row>
     <row r="21" spans="1:22" ht="16.5">
       <c r="A21" s="46"/>
-      <c r="B21" s="126" t="s">
+      <c r="B21" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="42" t="e">
+      <c r="C21" s="42">
         <f ca="1">[1]!GetColor(K6,C3:C20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D21" s="42" t="e">
+        <v>15</v>
+      </c>
+      <c r="D21" s="42">
         <f ca="1">[1]!GetColor(K6,D3:D20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E21" s="42" t="e">
+        <v>17</v>
+      </c>
+      <c r="E21" s="42">
         <f ca="1">[1]!GetColor(K6,E3:E20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F21" s="42" t="e">
+        <v>16</v>
+      </c>
+      <c r="F21" s="42">
         <f ca="1">[1]!GetColor(K6,F3:F20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G21" s="42" t="e">
+        <v>10</v>
+      </c>
+      <c r="G21" s="42">
         <f ca="1">[1]!GetColor(K6,G3:G20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H21" s="42" t="e">
+        <v>15</v>
+      </c>
+      <c r="H21" s="42">
         <f ca="1">[1]!GetColor(K6,H3:H20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I21" s="42" t="e">
+        <v>18</v>
+      </c>
+      <c r="I21" s="42">
         <f ca="1">[1]!GetColor(K6,I3:I20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J21" s="43" t="e">
+        <v>18</v>
+      </c>
+      <c r="J21" s="43">
         <f ca="1">SUM(C21:I21)</f>
-        <v>#NAME?</v>
+        <v>109</v>
       </c>
       <c r="K21" s="6"/>
       <c r="M21" s="2"/>
@@ -18429,38 +18604,38 @@
     </row>
     <row r="22" spans="1:22" ht="17.25" thickBot="1">
       <c r="A22" s="46"/>
-      <c r="B22" s="127"/>
-      <c r="C22" s="44" t="e">
+      <c r="B22" s="128"/>
+      <c r="C22" s="44">
         <f t="shared" ref="C22:I22" ca="1" si="0">C21/COUNTA(C3:C20)*100%</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D22" s="44" t="e">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="E22" s="44" t="e">
+        <v>0.94444444444444442</v>
+      </c>
+      <c r="E22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="F22" s="44" t="e">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G22" s="44" t="e">
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="G22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H22" s="44" t="e">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="H22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I22" s="44" t="e">
+        <v>1</v>
+      </c>
+      <c r="I22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="J22" s="45" t="e">
+        <v>1</v>
+      </c>
+      <c r="J22" s="45">
         <f ca="1">AVERAGE(C22:I22)</f>
-        <v>#NAME?</v>
+        <v>0.865079365079365</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="3"/>
@@ -18517,11 +18692,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G12" sqref="G11:G12"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -19154,40 +19329,40 @@
     </row>
     <row r="21" spans="1:22" ht="16.5">
       <c r="A21" s="46"/>
-      <c r="B21" s="126" t="s">
+      <c r="B21" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="42" t="e">
+      <c r="C21" s="42">
         <f ca="1">[1]!GetColor(K6,C3:C20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D21" s="42" t="e">
+        <v>16</v>
+      </c>
+      <c r="D21" s="42">
         <f ca="1">[1]!GetColor(K6,D3:D20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E21" s="42" t="e">
+        <v>14</v>
+      </c>
+      <c r="E21" s="42">
         <f ca="1">[1]!GetColor(K6,E3:E20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F21" s="42" t="e">
+        <v>12</v>
+      </c>
+      <c r="F21" s="42">
         <f ca="1">[1]!GetColor(K6,F3:F20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G21" s="42" t="e">
+        <v>9</v>
+      </c>
+      <c r="G21" s="42">
         <f ca="1">[1]!GetColor(K6,G3:G20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H21" s="42" t="e">
+        <v>4</v>
+      </c>
+      <c r="H21" s="42">
         <f ca="1">[1]!GetColor(K6,H3:H20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I21" s="42" t="e">
+        <v>0</v>
+      </c>
+      <c r="I21" s="42">
         <f ca="1">[1]!GetColor(K6,I3:I20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J21" s="43" t="e">
+        <v>0</v>
+      </c>
+      <c r="J21" s="43">
         <f ca="1">SUM(C21:I21)</f>
-        <v>#NAME?</v>
+        <v>55</v>
       </c>
       <c r="K21" s="6"/>
       <c r="M21" s="2"/>
@@ -19195,38 +19370,38 @@
     </row>
     <row r="22" spans="1:22" ht="17.25" thickBot="1">
       <c r="A22" s="46"/>
-      <c r="B22" s="127"/>
-      <c r="C22" s="44" t="e">
+      <c r="B22" s="128"/>
+      <c r="C22" s="44">
         <f t="shared" ref="C22:I22" ca="1" si="0">C21/COUNTA(C3:C20)*100%</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D22" s="44" t="e">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="D22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="E22" s="44" t="e">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="F22" s="44" t="e">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G22" s="44" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="G22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H22" s="44" t="e">
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="H22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I22" s="44" t="e">
+        <v>0</v>
+      </c>
+      <c r="I22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="J22" s="45" t="e">
+        <v>0</v>
+      </c>
+      <c r="J22" s="45">
         <f ca="1">AVERAGE(C22:I22)</f>
-        <v>#NAME?</v>
+        <v>0.43650793650793646</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="3"/>
@@ -19283,11 +19458,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -19425,13 +19600,13 @@
         <v>40</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F5" s="18" t="s">
         <v>40</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H5" s="17" t="s">
         <v>35</v>
@@ -19459,19 +19634,19 @@
         <v>40</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>40</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H6" s="17" t="s">
         <v>0</v>
       </c>
       <c r="I6" s="114" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J6" s="31"/>
       <c r="K6" s="87"/>
@@ -19484,17 +19659,17 @@
       <c r="B7" s="112">
         <v>0.4375</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="36" t="s">
         <v>62</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>62</v>
+      <c r="E7" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>63</v>
@@ -19503,7 +19678,7 @@
         <v>65</v>
       </c>
       <c r="I7" s="114" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J7" s="31"/>
       <c r="K7" s="89"/>
@@ -19516,17 +19691,17 @@
       <c r="B8" s="112">
         <v>0.47916666666666669</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="36" t="s">
         <v>62</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="17" t="s">
-        <v>62</v>
+      <c r="E8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="G8" s="17" t="s">
         <v>63</v>
@@ -19550,7 +19725,7 @@
       <c r="B9" s="112">
         <v>0.5</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="36" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="17" t="s">
@@ -19578,11 +19753,11 @@
       <c r="B10" s="112">
         <v>0.5625</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>18</v>
+      <c r="D10" s="125" t="s">
+        <v>49</v>
       </c>
       <c r="E10" s="125" t="s">
         <v>49</v>
@@ -19594,7 +19769,7 @@
         <v>18</v>
       </c>
       <c r="H10" s="115" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I10" s="18" t="s">
         <v>50</v>
@@ -19606,11 +19781,11 @@
       <c r="B11" s="112">
         <v>0.60416666666666663</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>18</v>
+      <c r="D11" s="125" t="s">
+        <v>49</v>
       </c>
       <c r="E11" s="125" t="s">
         <v>49</v>
@@ -19622,7 +19797,7 @@
         <v>18</v>
       </c>
       <c r="H11" s="115" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I11" s="18" t="s">
         <v>50</v>
@@ -19634,8 +19809,8 @@
       <c r="B12" s="112">
         <v>0.64583333333333337</v>
       </c>
-      <c r="C12" s="125" t="s">
-        <v>110</v>
+      <c r="C12" s="39" t="s">
+        <v>47</v>
       </c>
       <c r="D12" s="19" t="s">
         <v>18</v>
@@ -19665,8 +19840,8 @@
       <c r="B13" s="112">
         <v>0.6875</v>
       </c>
-      <c r="C13" s="125" t="s">
-        <v>111</v>
+      <c r="C13" s="124" t="s">
+        <v>110</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>18</v>
@@ -19696,8 +19871,8 @@
       <c r="B14" s="112">
         <v>0.72916666666666663</v>
       </c>
-      <c r="C14" s="125" t="s">
-        <v>111</v>
+      <c r="C14" s="124" t="s">
+        <v>110</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>18</v>
@@ -19727,7 +19902,7 @@
       <c r="B15" s="112">
         <v>0.75</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="36" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="17" t="s">
@@ -19759,20 +19934,20 @@
       <c r="B16" s="112">
         <v>0.79166666666666663</v>
       </c>
-      <c r="C16" s="125" t="s">
-        <v>111</v>
+      <c r="C16" s="39" t="s">
+        <v>109</v>
       </c>
       <c r="D16" s="125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>102</v>
       </c>
       <c r="F16" s="125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G16" s="125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H16" s="18" t="s">
         <v>50</v>
@@ -19793,20 +19968,20 @@
       <c r="B17" s="112">
         <v>0.83333333333333337</v>
       </c>
-      <c r="C17" s="125" t="s">
-        <v>111</v>
+      <c r="C17" s="39" t="s">
+        <v>109</v>
       </c>
       <c r="D17" s="125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>102</v>
       </c>
       <c r="F17" s="125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G17" s="125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H17" s="18" t="s">
         <v>50</v>
@@ -19825,7 +20000,7 @@
       <c r="B18" s="112">
         <v>0.875</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="36" t="s">
         <v>42</v>
       </c>
       <c r="D18" s="17" t="s">
@@ -19857,11 +20032,11 @@
       <c r="B19" s="112">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>50</v>
+      <c r="D19" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>50</v>
@@ -19889,7 +20064,7 @@
       <c r="B20" s="118">
         <v>0.95833333333333304</v>
       </c>
-      <c r="C20" s="121" t="s">
+      <c r="C20" s="126" t="s">
         <v>70</v>
       </c>
       <c r="D20" s="121" t="s">
@@ -19920,40 +20095,40 @@
     </row>
     <row r="21" spans="1:22" ht="16.5">
       <c r="A21" s="46"/>
-      <c r="B21" s="126" t="s">
+      <c r="B21" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="42" t="e">
+      <c r="C21" s="42">
         <f ca="1">[1]!GetColor(K6,C3:C20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D21" s="42" t="e">
+        <v>13</v>
+      </c>
+      <c r="D21" s="42">
         <f ca="1">[1]!GetColor(K6,D3:D20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E21" s="42" t="e">
+        <v>0</v>
+      </c>
+      <c r="E21" s="42">
         <f ca="1">[1]!GetColor(K6,E3:E20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F21" s="42" t="e">
+        <v>0</v>
+      </c>
+      <c r="F21" s="42">
         <f ca="1">[1]!GetColor(K6,F3:F20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G21" s="42" t="e">
+        <v>0</v>
+      </c>
+      <c r="G21" s="42">
         <f ca="1">[1]!GetColor(K6,G3:G20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="H21" s="42" t="e">
+        <v>0</v>
+      </c>
+      <c r="H21" s="42">
         <f ca="1">[1]!GetColor(K6,H3:H20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I21" s="42" t="e">
+        <v>0</v>
+      </c>
+      <c r="I21" s="42">
         <f ca="1">[1]!GetColor(K6,I3:I20, 0, 1) + NOW()*0</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J21" s="43" t="e">
+        <v>0</v>
+      </c>
+      <c r="J21" s="43">
         <f ca="1">SUM(C21:I21)</f>
-        <v>#NAME?</v>
+        <v>13</v>
       </c>
       <c r="K21" s="6"/>
       <c r="M21" s="2"/>
@@ -19961,38 +20136,38 @@
     </row>
     <row r="22" spans="1:22" ht="17.25" thickBot="1">
       <c r="A22" s="46"/>
-      <c r="B22" s="127"/>
-      <c r="C22" s="44" t="e">
+      <c r="B22" s="128"/>
+      <c r="C22" s="44">
         <f t="shared" ref="C22:I22" ca="1" si="0">C21/COUNTA(C3:C20)*100%</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D22" s="44" t="e">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="D22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="E22" s="44" t="e">
+        <v>0</v>
+      </c>
+      <c r="E22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="F22" s="44" t="e">
+        <v>0</v>
+      </c>
+      <c r="F22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="G22" s="44" t="e">
+        <v>0</v>
+      </c>
+      <c r="G22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="H22" s="44" t="e">
+        <v>0</v>
+      </c>
+      <c r="H22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I22" s="44" t="e">
+        <v>0</v>
+      </c>
+      <c r="I22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="J22" s="45" t="e">
+        <v>0</v>
+      </c>
+      <c r="J22" s="45">
         <f ca="1">AVERAGE(C22:I22)</f>
-        <v>#NAME?</v>
+        <v>0.10317460317460317</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="3"/>
@@ -20049,7 +20224,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="C3:J25"/>
   <sheetViews>
@@ -20074,9 +20249,9 @@
       <c r="C4" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="11" t="e">
+      <c r="D4" s="11">
         <f ca="1">'1周'!$J$21</f>
-        <v>#NAME?</v>
+        <v>0.89915966386554635</v>
       </c>
     </row>
     <row r="5" spans="3:10">
@@ -20202,9 +20377,9 @@
       <c r="C16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="11" t="e">
+      <c r="D16" s="11">
         <f ca="1">'1周'!$J$21</f>
-        <v>#NAME?</v>
+        <v>0.89915966386554635</v>
       </c>
       <c r="I16" s="9"/>
       <c r="J16" s="10"/>
@@ -20260,7 +20435,7 @@
       </c>
       <c r="D25" s="14" t="e">
         <f ca="1">AVERAGE(D4:D17)</f>
-        <v>#NAME?</v>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>
@@ -20271,7 +20446,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup type="stacked" displayEmptyCellsAs="gap">
+        <x14:sparklineGroup type="stacked" displayEmptyCellsAs="gap" xr2:uid="{00000000-0003-0000-0700-000000000000}">
           <x14:colorSeries rgb="FF0070C0"/>
           <x14:colorNegative rgb="FF000000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>

<commit_message>
today's plans are ready
</commit_message>
<xml_diff>
--- a/2020-21second.xlsx
+++ b/2020-21second.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AD7BED-F3C8-48D6-8AD4-91CAC6991323}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1周" sheetId="43" r:id="rId1"/>
@@ -29,17 +28,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'6周'!$B$2:$J$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'9周 '!$B$2:$J$22</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="I5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="I6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -71,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+    <comment ref="I7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -108,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+    <comment ref="I9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -124,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+    <comment ref="I10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -140,7 +139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
+    <comment ref="I11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -156,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
+    <comment ref="I12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -172,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
+    <comment ref="I13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -188,7 +187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
+    <comment ref="I15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -204,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
+    <comment ref="I16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -220,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
+    <comment ref="I18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -236,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000C000000}">
+    <comment ref="I19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -278,12 +277,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -299,7 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
+    <comment ref="D4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -315,7 +314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -331,7 +330,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -347,7 +346,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000005000000}">
+    <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -363,7 +362,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000006000000}">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -379,7 +378,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000007000000}">
+    <comment ref="D6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -395,7 +394,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000008000000}">
+    <comment ref="G6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -411,7 +410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000009000000}">
+    <comment ref="H6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -427,7 +426,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000A000000}">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -443,7 +442,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000B000000}">
+    <comment ref="G7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -459,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000C000000}">
+    <comment ref="I7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -476,7 +475,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000D000000}">
+    <comment ref="C8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -492,7 +491,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000E000000}">
+    <comment ref="G8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -508,7 +507,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00000F000000}">
+    <comment ref="I8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -545,7 +544,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000010000000}">
+    <comment ref="I9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -587,7 +586,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000011000000}">
+    <comment ref="C10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -603,7 +602,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000012000000}">
+    <comment ref="G10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -619,7 +618,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000013000000}">
+    <comment ref="H10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -635,7 +634,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000014000000}">
+    <comment ref="I10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -651,7 +650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000015000000}">
+    <comment ref="C11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -667,7 +666,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000016000000}">
+    <comment ref="G11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -683,7 +682,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000017000000}">
+    <comment ref="H11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -699,7 +698,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000018000000}">
+    <comment ref="I11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -715,7 +714,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000019000000}">
+    <comment ref="C12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -731,7 +730,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001A000000}">
+    <comment ref="G12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -747,7 +746,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001B000000}">
+    <comment ref="H12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -763,7 +762,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001C000000}">
+    <comment ref="I12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -779,7 +778,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001D000000}">
+    <comment ref="G13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -795,7 +794,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001E000000}">
+    <comment ref="H13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -811,7 +810,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00001F000000}">
+    <comment ref="I13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -827,7 +826,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000020000000}">
+    <comment ref="C14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -843,7 +842,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000021000000}">
+    <comment ref="G14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -859,7 +858,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000022000000}">
+    <comment ref="H14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -875,7 +874,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000023000000}">
+    <comment ref="I14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -891,7 +890,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000024000000}">
+    <comment ref="H15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -907,7 +906,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000025000000}">
+    <comment ref="I15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -924,7 +923,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000026000000}">
+    <comment ref="C16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -940,7 +939,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000027000000}">
+    <comment ref="G16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -956,7 +955,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000028000000}">
+    <comment ref="H16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -972,7 +971,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000029000000}">
+    <comment ref="I16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -988,7 +987,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002A000000}">
+    <comment ref="C17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1004,7 +1003,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002B000000}">
+    <comment ref="G17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1020,7 +1019,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002C000000}">
+    <comment ref="H17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1036,7 +1035,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002D000000}">
+    <comment ref="I17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1052,7 +1051,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002E000000}">
+    <comment ref="G18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1068,7 +1067,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-00002F000000}">
+    <comment ref="H18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1084,7 +1083,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000030000000}">
+    <comment ref="I18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1100,7 +1099,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000031000000}">
+    <comment ref="C19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1116,7 +1115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000032000000}">
+    <comment ref="G19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1132,7 +1131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000033000000}">
+    <comment ref="H19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1148,7 +1147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000034000000}">
+    <comment ref="I19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1164,7 +1163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000035000000}">
+    <comment ref="C20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1190,7 +1189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000036000000}">
+    <comment ref="G20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1206,7 +1205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000037000000}">
+    <comment ref="H20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1222,7 +1221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000038000000}">
+    <comment ref="I20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1243,12 +1242,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
+    <comment ref="C3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1264,7 +1263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1280,7 +1279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1296,7 +1295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
+    <comment ref="C4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1312,7 +1311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000005000000}">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1328,7 +1327,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000006000000}">
+    <comment ref="D5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1344,7 +1343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000007000000}">
+    <comment ref="E5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1360,7 +1359,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000008000000}">
+    <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1376,7 +1375,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000009000000}">
+    <comment ref="G5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1392,7 +1391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000A000000}">
+    <comment ref="H5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1408,7 +1407,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000B000000}">
+    <comment ref="C6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1424,7 +1423,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000C000000}">
+    <comment ref="D6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1440,7 +1439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000D000000}">
+    <comment ref="E6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1456,7 +1455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000E000000}">
+    <comment ref="F6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1472,7 +1471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00000F000000}">
+    <comment ref="G6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1488,7 +1487,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000010000000}">
+    <comment ref="H6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1504,7 +1503,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000011000000}">
+    <comment ref="C7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1520,7 +1519,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000012000000}">
+    <comment ref="D7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1536,7 +1535,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000013000000}">
+    <comment ref="E7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1552,7 +1551,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000014000000}">
+    <comment ref="F7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1568,7 +1567,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000015000000}">
+    <comment ref="G7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1584,7 +1583,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000016000000}">
+    <comment ref="I7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1601,7 +1600,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000017000000}">
+    <comment ref="C8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1617,7 +1616,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000018000000}">
+    <comment ref="D8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1633,7 +1632,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000019000000}">
+    <comment ref="E8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1649,7 +1648,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00001A000000}">
+    <comment ref="F8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1665,7 +1664,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00001B000000}">
+    <comment ref="G8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1681,7 +1680,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00001C000000}">
+    <comment ref="I8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1718,7 +1717,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00001D000000}">
+    <comment ref="E9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1734,7 +1733,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00001E000000}">
+    <comment ref="F9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1750,7 +1749,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00001F000000}">
+    <comment ref="I9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1792,7 +1791,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000020000000}">
+    <comment ref="C10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1808,7 +1807,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000021000000}">
+    <comment ref="D10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1824,7 +1823,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000022000000}">
+    <comment ref="E10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1840,7 +1839,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000023000000}">
+    <comment ref="F10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1856,7 +1855,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000024000000}">
+    <comment ref="G10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1872,7 +1871,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000025000000}">
+    <comment ref="H10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1888,7 +1887,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000026000000}">
+    <comment ref="I10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1904,7 +1903,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000027000000}">
+    <comment ref="C11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1920,7 +1919,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000028000000}">
+    <comment ref="D11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1936,7 +1935,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000029000000}">
+    <comment ref="F11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1952,7 +1951,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00002A000000}">
+    <comment ref="G11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1968,7 +1967,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00002B000000}">
+    <comment ref="H11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -1984,7 +1983,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00002C000000}">
+    <comment ref="I11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2000,7 +1999,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00002D000000}">
+    <comment ref="C12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2016,7 +2015,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00002E000000}">
+    <comment ref="D12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2032,7 +2031,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00002F000000}">
+    <comment ref="E12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2048,7 +2047,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000030000000}">
+    <comment ref="F12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2064,7 +2063,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000031000000}">
+    <comment ref="G12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2080,7 +2079,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000032000000}">
+    <comment ref="H12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2096,7 +2095,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000033000000}">
+    <comment ref="I12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2112,7 +2111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000034000000}">
+    <comment ref="C13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2128,7 +2127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000035000000}">
+    <comment ref="D13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2144,7 +2143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000036000000}">
+    <comment ref="E13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2160,7 +2159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000037000000}">
+    <comment ref="F13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2176,7 +2175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000038000000}">
+    <comment ref="G13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2192,7 +2191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000039000000}">
+    <comment ref="H13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2208,7 +2207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00003A000000}">
+    <comment ref="I13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2224,7 +2223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00003B000000}">
+    <comment ref="C14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2240,7 +2239,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00003C000000}">
+    <comment ref="D14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2256,7 +2255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00003D000000}">
+    <comment ref="E14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2272,7 +2271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00003E000000}">
+    <comment ref="F14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2288,7 +2287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00003F000000}">
+    <comment ref="G14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2304,7 +2303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000040000000}">
+    <comment ref="H14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2320,7 +2319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000041000000}">
+    <comment ref="I14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2336,7 +2335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000042000000}">
+    <comment ref="H15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2352,7 +2351,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000043000000}">
+    <comment ref="I15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2369,7 +2368,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000044000000}">
+    <comment ref="C16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2385,7 +2384,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000045000000}">
+    <comment ref="D16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2401,7 +2400,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000046000000}">
+    <comment ref="F16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2417,7 +2416,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000047000000}">
+    <comment ref="G16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2433,7 +2432,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000048000000}">
+    <comment ref="H16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2449,7 +2448,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000049000000}">
+    <comment ref="I16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2465,7 +2464,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00004A000000}">
+    <comment ref="C17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2481,7 +2480,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00004B000000}">
+    <comment ref="D17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2497,7 +2496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00004C000000}">
+    <comment ref="G17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2513,7 +2512,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00004D000000}">
+    <comment ref="H17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2529,7 +2528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00004E000000}">
+    <comment ref="I17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2545,7 +2544,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00004F000000}">
+    <comment ref="D18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2561,7 +2560,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000050000000}">
+    <comment ref="E18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2577,7 +2576,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000051000000}">
+    <comment ref="F18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2593,7 +2592,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000052000000}">
+    <comment ref="G18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2609,7 +2608,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000053000000}">
+    <comment ref="H18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2625,7 +2624,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000054000000}">
+    <comment ref="I18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2641,7 +2640,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000055000000}">
+    <comment ref="C19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2657,7 +2656,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000056000000}">
+    <comment ref="E19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2673,7 +2672,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000057000000}">
+    <comment ref="F19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2689,7 +2688,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000058000000}">
+    <comment ref="G19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2705,7 +2704,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000059000000}">
+    <comment ref="H19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2721,7 +2720,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00005A000000}">
+    <comment ref="I19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2737,7 +2736,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00005B000000}">
+    <comment ref="C20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2753,7 +2752,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00005C000000}">
+    <comment ref="E20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2769,7 +2768,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00005D000000}">
+    <comment ref="F20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2785,7 +2784,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-00005E000000}">
+    <comment ref="G20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2806,12 +2805,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>作者</author>
   </authors>
   <commentList>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
+    <comment ref="E3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2827,7 +2826,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2843,7 +2842,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000003000000}">
+    <comment ref="H3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2859,7 +2858,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000004000000}">
+    <comment ref="H4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2875,7 +2874,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000005000000}">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2891,7 +2890,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000006000000}">
+    <comment ref="D5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+Dirac的量子力学原理。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2907,7 +2922,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000007000000}">
+    <comment ref="F5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2923,7 +2938,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000008000000}">
+    <comment ref="G5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2939,7 +2954,55 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000009000000}">
+    <comment ref="H5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+看量子力学放松一下，当然是Dirac的咯，一口气推完置换部分吧</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+原本是想在数值上实现的，但不得不重新推导了。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+Dirac的量子力学原理。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -2955,39 +3018,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000A000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-看量子力学放松一下，当然是Dirac的咯，一口气推完置换部分吧</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000B000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-原本是想在数值上实现的，但不得不重新推导了。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000C000000}">
+    <comment ref="F6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3003,7 +3034,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000D000000}">
+    <comment ref="G6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3019,39 +3050,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000E000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-Dirac的量子力学讲义。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00000F000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-Dirac的量子力学讲义。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000010000000}">
+    <comment ref="I6" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3088,7 +3087,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{73E161C9-2E85-47BA-A021-8842B7C97393}">
+    <comment ref="E7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3104,7 +3103,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{B243C8A6-BAFB-4ECB-8349-4F4A49FA1F46}">
+    <comment ref="F7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3120,7 +3119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000011000000}">
+    <comment ref="I7" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3157,7 +3156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{C558CCFF-D288-4C59-9F45-12C2FDB369DC}">
+    <comment ref="E8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3173,7 +3172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{9D04EB6E-6470-4E02-9A9E-1023E054A0DC}">
+    <comment ref="F8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3189,7 +3188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000012000000}">
+    <comment ref="I8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3205,7 +3204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000013000000}">
+    <comment ref="E9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3221,7 +3220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000014000000}">
+    <comment ref="F9" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3237,7 +3236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000015000000}">
+    <comment ref="C10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3253,7 +3252,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{D46F7D6A-E363-4DEE-9A8C-5F6F779B6667}">
+    <comment ref="D10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3269,39 +3268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000017000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-还是那篇综述。一口气翻译完吧。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000018000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-得去1教进行开题报告。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000019000000}">
+    <comment ref="E10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3317,7 +3284,39 @@
         </r>
       </text>
     </comment>
-    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00001A000000}">
+    <comment ref="F10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+尝试非周期方向，各种尝试。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+尝试非周期方向，各种尝试。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3333,7 +3332,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00001B000000}">
+    <comment ref="I10" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3349,7 +3348,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00001C000000}">
+    <comment ref="C11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3365,7 +3364,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{A9059024-5895-4F21-8FEC-07A1B1501261}">
+    <comment ref="D11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3381,23 +3380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00001E000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-得去1教进行开题报告。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00001F000000}">
+    <comment ref="E11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3413,7 +3396,39 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000020000000}">
+    <comment ref="F11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+尝试非周期方向，各种尝试。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+尝试非周期方向，各种尝试。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3429,7 +3444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000021000000}">
+    <comment ref="I11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3445,7 +3460,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{4E890EBE-FBF4-42B9-846C-32B34D3DD992}">
+    <comment ref="C12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3461,7 +3476,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000023000000}">
+    <comment ref="D12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+和老师讨论之后，对任务进一步推进。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3477,7 +3508,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000024000000}">
+    <comment ref="F12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3493,7 +3524,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000025000000}">
+    <comment ref="G12" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3509,7 +3540,87 @@
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000026000000}">
+    <comment ref="H12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+还是玩那个游戏。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+还是玩那个游戏。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+八卦去了。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+完成一些和哈密顿量相关的事情。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+重新写代码。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3525,7 +3636,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000027000000}">
+    <comment ref="G13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+尝试非周期方向，各种尝试。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3541,7 +3668,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000028000000}">
+    <comment ref="I13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3557,7 +3684,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{277309F2-30DC-4FCB-A3B5-3B6CFDDBAB61}">
+    <comment ref="C14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3573,7 +3700,39 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000029000000}">
+    <comment ref="D14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+如果没有其它事情，我需要进行一下代码的维护。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+重新写代码。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3589,7 +3748,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00002A000000}">
+    <comment ref="G14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3605,39 +3764,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00002B000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-尝试非周期方向，各种尝试。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00002C000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-尝试非周期方向，各种尝试。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00002D000000}">
+    <comment ref="H14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3653,7 +3780,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00002E000000}">
+    <comment ref="I14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3669,119 +3796,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{7872573E-29A9-4B86-B1DD-9683A03FD836}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-八卦去了。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00002F000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-尝试非周期方向，各种尝试。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000030000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-尝试非周期方向，各种尝试。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000031000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-尝试非周期方向，各种尝试。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000032000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-尝试非周期方向，各种尝试。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000033000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-还是玩那个游戏。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000034000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-还是玩那个游戏。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000035000000}">
+    <comment ref="I15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3798,7 +3813,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{755D3773-871E-4493-A4CB-E67E905F830B}">
+    <comment ref="C16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3814,7 +3829,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000036000000}">
+    <comment ref="D16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+代码维护应该还是要花一些时间。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3830,7 +3861,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000037000000}">
+    <comment ref="G16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3846,7 +3877,71 @@
         </r>
       </text>
     </comment>
-    <comment ref="G16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000038000000}">
+    <comment ref="H16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+还是玩那个游戏。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I16" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+还是玩那个游戏。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+完成了新的小量推导。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+维护完了可以联系王沛正，谈谈网站的事情。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3862,7 +3957,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="H16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000039000000}">
+    <comment ref="G17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="11"/>
+            <color indexed="81"/>
+            <rFont val="华文楷体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>作者:
+重新写代码。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3878,7 +3989,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00003A000000}">
+    <comment ref="I17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3894,119 +4005,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{A951F08F-EC50-4584-A17D-47B20FDBF644}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-完成了新的小量推导。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00003B000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-重新写代码。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00003C000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-重新写代码。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00003D000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-重新写代码。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00003E000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-还是玩那个游戏。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00003F000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-还是玩那个游戏。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000040000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="11"/>
-            <color indexed="81"/>
-            <rFont val="华文楷体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>作者:
-清理伤口。</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000041000000}">
+    <comment ref="E18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4022,7 +4021,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000042000000}">
+    <comment ref="F18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4038,7 +4037,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000043000000}">
+    <comment ref="G18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4054,7 +4053,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000044000000}">
+    <comment ref="H18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4070,7 +4069,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000045000000}">
+    <comment ref="I18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4086,7 +4085,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{AECCB75A-6506-4A14-89C1-40F5223FF2B7}">
+    <comment ref="D19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4102,7 +4101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000046000000}">
+    <comment ref="E19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4118,7 +4117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000047000000}">
+    <comment ref="F19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4134,7 +4133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000048000000}">
+    <comment ref="G19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4150,7 +4149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000049000000}">
+    <comment ref="H19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4166,7 +4165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00004A000000}">
+    <comment ref="I19" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4182,7 +4181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00004B000000}">
+    <comment ref="E20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4198,7 +4197,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00004C000000}">
+    <comment ref="F20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4214,7 +4213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-00004D000000}">
+    <comment ref="G20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -4235,7 +4234,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="115">
   <si>
     <t>起床吃饭</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -4701,11 +4700,15 @@
     <t>联系好友</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>代码维护</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="26">
     <font>
       <sz val="11"/>
@@ -5909,7 +5912,7 @@
   <cellStyles count="3">
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="样式 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="样式 1" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -8620,6 +8623,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -8674,10 +8678,10 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.72222222222222221</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.5555555555555552E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -14731,23 +14735,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -14783,23 +14770,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -14975,7 +14945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O23"/>
   <sheetViews>
@@ -15707,7 +15677,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -16438,7 +16408,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -17182,7 +17152,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
@@ -17926,7 +17896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
@@ -18692,7 +18662,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -19458,11 +19428,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -19531,7 +19501,7 @@
       <c r="C3" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="70" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="17" t="s">
@@ -19564,7 +19534,7 @@
       <c r="C4" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="37" t="s">
         <v>89</v>
       </c>
       <c r="E4" s="18" t="s">
@@ -19759,11 +19729,11 @@
       <c r="D10" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="125" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="125" t="s">
-        <v>69</v>
+      <c r="E10" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>18</v>
@@ -19787,11 +19757,11 @@
       <c r="D11" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="125" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="125" t="s">
-        <v>69</v>
+      <c r="E11" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="G11" s="19" t="s">
         <v>18</v>
@@ -19846,8 +19816,8 @@
       <c r="D13" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="19" t="s">
-        <v>18</v>
+      <c r="E13" s="125" t="s">
+        <v>110</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>18</v>
@@ -19875,10 +19845,10 @@
         <v>110</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>18</v>
+        <v>114</v>
+      </c>
+      <c r="E14" s="125" t="s">
+        <v>110</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>18</v>
@@ -19937,8 +19907,8 @@
       <c r="C16" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="D16" s="125" t="s">
-        <v>110</v>
+      <c r="D16" s="19" t="s">
+        <v>114</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>102</v>
@@ -19971,8 +19941,8 @@
       <c r="C17" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="125" t="s">
-        <v>110</v>
+      <c r="D17" s="19" t="s">
+        <v>114</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>102</v>
@@ -20032,7 +20002,7 @@
       <c r="B19" s="112">
         <v>0.91666666666666663</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="49" t="s">
         <v>50</v>
       </c>
       <c r="D19" s="17" t="s">
@@ -20100,11 +20070,11 @@
       </c>
       <c r="C21" s="42">
         <f ca="1">[1]!GetColor(K6,C3:C20, 0, 1) + NOW()*0</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="42">
         <f ca="1">[1]!GetColor(K6,D3:D20, 0, 1) + NOW()*0</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="42">
         <f ca="1">[1]!GetColor(K6,E3:E20, 0, 1) + NOW()*0</f>
@@ -20139,11 +20109,11 @@
       <c r="B22" s="128"/>
       <c r="C22" s="44">
         <f t="shared" ref="C22:I22" ca="1" si="0">C21/COUNTA(C3:C20)*100%</f>
-        <v>0.72222222222222221</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D22" s="44">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>5.5555555555555552E-2</v>
       </c>
       <c r="E22" s="44">
         <f t="shared" ca="1" si="0"/>
@@ -20224,7 +20194,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="C3:J25"/>
   <sheetViews>
@@ -20446,7 +20416,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x14:sparklineGroup type="stacked" displayEmptyCellsAs="gap" xr2:uid="{00000000-0003-0000-0700-000000000000}">
+        <x14:sparklineGroup type="stacked" displayEmptyCellsAs="gap">
           <x14:colorSeries rgb="FF0070C0"/>
           <x14:colorNegative rgb="FF000000"/>
           <x14:colorAxis rgb="FF000000"/>

</xml_diff>